<commit_message>
data: increase quiz data points
</commit_message>
<xml_diff>
--- a/data/quiz.xlsx
+++ b/data/quiz.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yiqiling/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yiqiling/Documents/GitHub/bronze-clocks/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{541DDE79-FDC9-2742-B750-D99E30CE2178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B85BBF1-6B73-EF4C-983F-34161B35D62B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14080" yWindow="4280" windowWidth="24320" windowHeight="17320" xr2:uid="{CBACCA3D-7D51-594C-9FE5-F6151FA40A1D}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="124">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -471,6 +471,49 @@
   </si>
   <si>
     <t>https://apiwenwu.hebeimuseum.org.cn/news/show/id/17.html</t>
+  </si>
+  <si>
+    <t>大盂鼎</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>大克鼎</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Da Ke Ding</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.shanghaimuseum.net/resource/museum_files/show_files/20151104094055028/index.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ritual Cauldron (Ding) of Duke Ke</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fufeng, Shaanxi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>static/images/大克鼎.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>static/images/大盂鼎.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Da Yu Ding</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ritual Cauldron (Ding) of Duke Yu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.chnmuseum.cn/portals/0/web/zt/202106dayuding/</t>
   </si>
 </sst>
 </file>
@@ -850,10 +893,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2871DCE2-55FD-4844-8A79-74A725EB9D9C}">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" zoomScale="81" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1446,6 +1489,70 @@
         <v>112</v>
       </c>
     </row>
+    <row r="19" spans="1:10">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>113</v>
+      </c>
+      <c r="C19" t="s">
+        <v>121</v>
+      </c>
+      <c r="D19" t="s">
+        <v>122</v>
+      </c>
+      <c r="E19" t="s">
+        <v>50</v>
+      </c>
+      <c r="F19" t="s">
+        <v>70</v>
+      </c>
+      <c r="G19">
+        <v>-1040</v>
+      </c>
+      <c r="H19">
+        <v>-1003</v>
+      </c>
+      <c r="I19" t="s">
+        <v>120</v>
+      </c>
+      <c r="J19" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>114</v>
+      </c>
+      <c r="C20" t="s">
+        <v>115</v>
+      </c>
+      <c r="D20" t="s">
+        <v>117</v>
+      </c>
+      <c r="E20" t="s">
+        <v>118</v>
+      </c>
+      <c r="F20" t="s">
+        <v>34</v>
+      </c>
+      <c r="G20">
+        <v>-950</v>
+      </c>
+      <c r="H20">
+        <v>-886</v>
+      </c>
+      <c r="I20" t="s">
+        <v>119</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
@@ -1453,6 +1560,7 @@
     <hyperlink ref="J5" r:id="rId2" xr:uid="{F6AC1975-F65F-954C-BBA0-B25006D8EA93}"/>
     <hyperlink ref="J6" r:id="rId3" xr:uid="{FDFBAC33-9B07-F74A-92B2-FDB544E92443}"/>
     <hyperlink ref="J8" r:id="rId4" location="inline_content_intro" xr:uid="{BC9A64A1-DC3B-E74D-95A9-B7BFD1D24100}"/>
+    <hyperlink ref="J20" r:id="rId5" xr:uid="{6C482A1F-3701-B14B-9FBA-971BC5FA0820}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: develop color module
</commit_message>
<xml_diff>
--- a/data/quiz.xlsx
+++ b/data/quiz.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yiqiling/Documents/GitHub/bronze-clocks/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{140326FC-DB1A-294A-801B-7F0A61A77FA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE57E3F0-D4E4-D047-BA85-0C07BFA7D7E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5080" yWindow="1800" windowWidth="24320" windowHeight="17320" xr2:uid="{CBACCA3D-7D51-594C-9FE5-F6151FA40A1D}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{CBACCA3D-7D51-594C-9FE5-F6151FA40A1D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="140">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -556,6 +556,25 @@
   </si>
   <si>
     <t>Fang Yi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>错金嵌松石樽</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Wine Vessel (Zun) with Gold-inlaid Turquoise </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cuo Jin Qian Song Shi Zun</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.dpm.org.cn/collection/bronze/229985.html</t>
+  </si>
+  <si>
+    <t>static/images/错金嵌松石樽.png</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -936,10 +955,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2871DCE2-55FD-4844-8A79-74A725EB9D9C}">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="81" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1660,6 +1679,38 @@
         <v>130</v>
       </c>
     </row>
+    <row r="23" spans="1:10">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>135</v>
+      </c>
+      <c r="C23" t="s">
+        <v>137</v>
+      </c>
+      <c r="D23" t="s">
+        <v>136</v>
+      </c>
+      <c r="E23" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" t="s">
+        <v>36</v>
+      </c>
+      <c r="G23">
+        <v>-330</v>
+      </c>
+      <c r="H23">
+        <v>-221</v>
+      </c>
+      <c r="I23" t="s">
+        <v>139</v>
+      </c>
+      <c r="J23" t="s">
+        <v>138</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>

</xml_diff>